<commit_message>
Exported figures as png
</commit_message>
<xml_diff>
--- a/results/CO2_reduction_100_percent.xlsx
+++ b/results/CO2_reduction_100_percent.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="47">
   <si>
     <t>cluster_0</t>
   </si>
@@ -567,28 +567,28 @@
         <v>25</v>
       </c>
       <c r="D2">
-        <v>0.2642231213900008</v>
+        <v>0.2642231213900199</v>
       </c>
       <c r="E2">
-        <v>0.2537514178015767</v>
+        <v>0.2537514178015782</v>
       </c>
       <c r="F2">
-        <v>0.1767485276706301</v>
+        <v>0.1767485276706169</v>
       </c>
       <c r="G2">
-        <v>0.2441622324083482</v>
+        <v>0.2441622324082958</v>
       </c>
       <c r="H2">
-        <v>0.3514525396472772</v>
+        <v>0.3514525396472714</v>
       </c>
       <c r="I2">
-        <v>0.1555942174877734</v>
+        <v>0.1555942174877632</v>
       </c>
       <c r="J2">
-        <v>0.1648731255889925</v>
+        <v>0.1648731255889077</v>
       </c>
       <c r="K2">
-        <v>0.06598481800539893</v>
+        <v>0.06598481800541314</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -600,28 +600,28 @@
         <v>25</v>
       </c>
       <c r="D3">
-        <v>0.2642231213900008</v>
+        <v>0.2642231213900199</v>
       </c>
       <c r="E3">
-        <v>0.2537514178015767</v>
+        <v>0.2537514178015782</v>
       </c>
       <c r="F3">
-        <v>0.1767485276706301</v>
+        <v>0.1767485276706169</v>
       </c>
       <c r="G3">
-        <v>0.2441622324083482</v>
+        <v>0.2441622324082958</v>
       </c>
       <c r="H3">
-        <v>0.3514525396472772</v>
+        <v>0.3514525396472714</v>
       </c>
       <c r="I3">
-        <v>0.1555942174877734</v>
+        <v>0.1555942174877632</v>
       </c>
       <c r="J3">
-        <v>0.1648731255889925</v>
+        <v>0.1648731255889077</v>
       </c>
       <c r="K3">
-        <v>0.06598481800539893</v>
+        <v>0.06598481800541314</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -633,28 +633,28 @@
         <v>26</v>
       </c>
       <c r="D4">
-        <v>4884.879300979863</v>
+        <v>4884.879300980216</v>
       </c>
       <c r="E4">
-        <v>4691.281527113639</v>
+        <v>4691.281527113666</v>
       </c>
       <c r="F4">
-        <v>3267.674758192459</v>
+        <v>3267.674758192215</v>
       </c>
       <c r="G4">
-        <v>4513.999489893663</v>
+        <v>4513.999489892694</v>
       </c>
       <c r="H4">
-        <v>6497.551111985159</v>
+        <v>6497.551111985052</v>
       </c>
       <c r="I4">
-        <v>2876.580097758799</v>
+        <v>2876.580097758609</v>
       </c>
       <c r="J4">
-        <v>3048.125819726244</v>
+        <v>3048.125819724676</v>
       </c>
       <c r="K4">
-        <v>1219.907894350137</v>
+        <v>1219.9078943504</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -664,28 +664,28 @@
         <v>27</v>
       </c>
       <c r="D5">
-        <v>4884.879300979863</v>
+        <v>4884.879300980216</v>
       </c>
       <c r="E5">
-        <v>4691.281527113639</v>
+        <v>4691.281527113666</v>
       </c>
       <c r="F5">
-        <v>3267.674758192459</v>
+        <v>3267.674758192215</v>
       </c>
       <c r="G5">
-        <v>4513.999489893663</v>
+        <v>4513.999489892694</v>
       </c>
       <c r="H5">
-        <v>6497.551111985159</v>
+        <v>6497.551111985052</v>
       </c>
       <c r="I5">
-        <v>2876.580097758799</v>
+        <v>2876.580097758609</v>
       </c>
       <c r="J5">
-        <v>3048.125819726244</v>
+        <v>3048.125819724676</v>
       </c>
       <c r="K5">
-        <v>1219.907894350137</v>
+        <v>1219.9078943504</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -699,28 +699,28 @@
         <v>28</v>
       </c>
       <c r="D6">
-        <v>133963.4514329218</v>
+        <v>133963.4514329197</v>
       </c>
       <c r="E6">
-        <v>66115.98745484417</v>
+        <v>66115.98745484406</v>
       </c>
       <c r="F6">
-        <v>124796.7594675441</v>
+        <v>124796.759467546</v>
       </c>
       <c r="G6">
-        <v>40441.20326623051</v>
+        <v>40441.20326623064</v>
       </c>
       <c r="H6">
-        <v>77229.28116530157</v>
+        <v>77229.28116530248</v>
       </c>
       <c r="I6">
-        <v>41413.40915452756</v>
+        <v>41413.40915452744</v>
       </c>
       <c r="J6">
-        <v>28088.76622265798</v>
+        <v>28088.76622265801</v>
       </c>
       <c r="K6">
-        <v>15851.14124473496</v>
+        <v>15851.14124473505</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -730,28 +730,28 @@
         <v>29</v>
       </c>
       <c r="D7">
-        <v>133963.4514329218</v>
+        <v>133963.4514329197</v>
       </c>
       <c r="E7">
-        <v>66115.98745484417</v>
+        <v>66115.98745484406</v>
       </c>
       <c r="F7">
-        <v>124796.7594675441</v>
+        <v>124796.759467546</v>
       </c>
       <c r="G7">
-        <v>40441.20326623051</v>
+        <v>40441.20326623064</v>
       </c>
       <c r="H7">
-        <v>77229.28116530157</v>
+        <v>77229.28116530248</v>
       </c>
       <c r="I7">
-        <v>41413.40915452756</v>
+        <v>41413.40915452744</v>
       </c>
       <c r="J7">
-        <v>28088.76622265798</v>
+        <v>28088.76622265801</v>
       </c>
       <c r="K7">
-        <v>15851.14124473496</v>
+        <v>15851.14124473505</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -825,22 +825,22 @@
         <v>28</v>
       </c>
       <c r="D10">
-        <v>3167.329183065777</v>
+        <v>3167.329183065871</v>
       </c>
       <c r="E10">
-        <v>170.9880017507264</v>
+        <v>170.988001750725</v>
       </c>
       <c r="F10">
-        <v>174.4775528077582</v>
+        <v>174.4775528077909</v>
       </c>
       <c r="G10">
-        <v>198.9044102033907</v>
+        <v>198.9044102034098</v>
       </c>
       <c r="H10">
-        <v>12204.71027128419</v>
+        <v>12204.71027128515</v>
       </c>
       <c r="K10">
-        <v>1480.823705210843</v>
+        <v>1480.823705210851</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -850,22 +850,22 @@
         <v>29</v>
       </c>
       <c r="D11">
-        <v>3167.329183065777</v>
+        <v>3167.329183065871</v>
       </c>
       <c r="E11">
-        <v>170.9880017507264</v>
+        <v>170.988001750725</v>
       </c>
       <c r="F11">
-        <v>174.4775528077582</v>
+        <v>174.4775528077909</v>
       </c>
       <c r="G11">
-        <v>198.9044102033907</v>
+        <v>198.9044102034098</v>
       </c>
       <c r="H11">
-        <v>12204.71027128419</v>
+        <v>12204.71027128515</v>
       </c>
       <c r="K11">
-        <v>1480.823705210843</v>
+        <v>1480.823705210851</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -906,28 +906,28 @@
         <v>31</v>
       </c>
       <c r="D13">
-        <v>15855.22909103999</v>
+        <v>15855.22909103749</v>
       </c>
       <c r="E13">
-        <v>11007.05688237806</v>
+        <v>11007.0568823791</v>
       </c>
       <c r="F13">
-        <v>16452.59494376484</v>
+        <v>16452.59494376374</v>
       </c>
       <c r="G13">
-        <v>5264.131864364819</v>
+        <v>5264.131864365728</v>
       </c>
       <c r="H13">
-        <v>10078.26752509824</v>
+        <v>10078.26752509777</v>
       </c>
       <c r="I13">
-        <v>5747.423572107636</v>
+        <v>5747.423572108148</v>
       </c>
       <c r="J13">
-        <v>3710.050513811987</v>
+        <v>3710.050513811419</v>
       </c>
       <c r="K13">
-        <v>1453.124166487185</v>
+        <v>1453.124166487049</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -937,28 +937,28 @@
         <v>32</v>
       </c>
       <c r="D14">
-        <v>15855.22909103999</v>
+        <v>15855.22909103749</v>
       </c>
       <c r="E14">
-        <v>11007.05688237806</v>
+        <v>11007.0568823791</v>
       </c>
       <c r="F14">
-        <v>16452.59494376484</v>
+        <v>16452.59494376374</v>
       </c>
       <c r="G14">
-        <v>5264.131864364819</v>
+        <v>5264.131864365728</v>
       </c>
       <c r="H14">
-        <v>10078.26752509824</v>
+        <v>10078.26752509777</v>
       </c>
       <c r="I14">
-        <v>5747.423572107636</v>
+        <v>5747.423572108148</v>
       </c>
       <c r="J14">
-        <v>3710.050513811987</v>
+        <v>3710.050513811419</v>
       </c>
       <c r="K14">
-        <v>1453.124166487185</v>
+        <v>1453.124166487049</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -972,7 +972,7 @@
         <v>25</v>
       </c>
       <c r="D15">
-        <v>3.094442683017956</v>
+        <v>3.093174765840486</v>
       </c>
       <c r="E15">
         <v>1.909966851869815</v>
@@ -1005,7 +1005,7 @@
         <v>30</v>
       </c>
       <c r="D16">
-        <v>41.87836191150959</v>
+        <v>41.86120266835304</v>
       </c>
       <c r="E16">
         <v>25.84836471541348</v>
@@ -1038,7 +1038,7 @@
         <v>25</v>
       </c>
       <c r="D17">
-        <v>2.550023978168331</v>
+        <v>2.548979131151897</v>
       </c>
       <c r="E17">
         <v>1.57393811056944</v>
@@ -1071,7 +1071,7 @@
         <v>33</v>
       </c>
       <c r="D18">
-        <v>27.22093524248123</v>
+        <v>27.20978173442948</v>
       </c>
       <c r="E18">
         <v>16.80143706501876</v>
@@ -1104,28 +1104,28 @@
         <v>28</v>
       </c>
       <c r="D19">
-        <v>43565.08243798192</v>
+        <v>41852.37878794894</v>
       </c>
       <c r="E19">
-        <v>22702.64148823543</v>
+        <v>22946.92167731431</v>
       </c>
       <c r="F19">
-        <v>33592.67633640656</v>
+        <v>35183.7468718614</v>
       </c>
       <c r="G19">
-        <v>18866.7994772524</v>
+        <v>18918.59115568295</v>
       </c>
       <c r="H19">
-        <v>25522.49914256721</v>
+        <v>28552.53971878443</v>
       </c>
       <c r="I19">
-        <v>18593.05120575628</v>
+        <v>18657.07905438971</v>
       </c>
       <c r="J19">
-        <v>12920.97807013702</v>
+        <v>12920.97807013712</v>
       </c>
       <c r="K19">
-        <v>4754.050637194372</v>
+        <v>4848.886320037049</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1135,28 +1135,28 @@
         <v>29</v>
       </c>
       <c r="D20">
-        <v>43565.08243798192</v>
+        <v>41852.37878794894</v>
       </c>
       <c r="E20">
-        <v>22702.64148823543</v>
+        <v>22946.92167731431</v>
       </c>
       <c r="F20">
-        <v>33592.67633640656</v>
+        <v>35183.7468718614</v>
       </c>
       <c r="G20">
-        <v>18866.7994772524</v>
+        <v>18918.59115568295</v>
       </c>
       <c r="H20">
-        <v>25522.49914256721</v>
+        <v>28552.53971878443</v>
       </c>
       <c r="I20">
-        <v>18593.05120575628</v>
+        <v>18657.07905438971</v>
       </c>
       <c r="J20">
-        <v>12920.97807013702</v>
+        <v>12920.97807013712</v>
       </c>
       <c r="K20">
-        <v>4754.050637194372</v>
+        <v>4848.886320037049</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1168,7 +1168,7 @@
         <v>25</v>
       </c>
       <c r="D21">
-        <v>0.5444187048496246</v>
+        <v>0.5441956346885896</v>
       </c>
       <c r="E21">
         <v>0.3360287413003753</v>
@@ -1299,16 +1299,16 @@
         <v>28</v>
       </c>
       <c r="E26">
-        <v>14775.89716598765</v>
+        <v>14775.8971659878</v>
       </c>
       <c r="F26">
-        <v>220191.9529009698</v>
+        <v>219332.5987403445</v>
       </c>
       <c r="G26">
-        <v>22383.59148159905</v>
+        <v>21902.92327745889</v>
       </c>
       <c r="J26">
-        <v>74853.64465283373</v>
+        <v>74884.7284241693</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1318,16 +1318,16 @@
         <v>29</v>
       </c>
       <c r="E27">
-        <v>14775.89716598765</v>
+        <v>14775.8971659878</v>
       </c>
       <c r="F27">
-        <v>220191.9529009698</v>
+        <v>219332.5987403445</v>
       </c>
       <c r="G27">
-        <v>22383.59148159905</v>
+        <v>21902.92327745889</v>
       </c>
       <c r="J27">
-        <v>74853.64465283373</v>
+        <v>74884.7284241693</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1368,19 +1368,19 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1.97645004902914</v>
+        <v>1.986361954635187</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0.258887642071748</v>
+        <v>0.2553185243851415</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29">
-        <v>3.688291157622347</v>
+        <v>3.682132470237111</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -1401,19 +1401,19 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>14.74550842531224</v>
+        <v>14.8194572143022</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>1.931457822196596</v>
+        <v>1.904830053412539</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
-        <v>27.51687469482973</v>
+        <v>27.4709271755527</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -1434,19 +1434,19 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>1.652048863672271</v>
+        <v>1.660333895920538</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0.2163955699834229</v>
+        <v>0.2134122632100657</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>3.082919914336093</v>
+        <v>3.077772072374951</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -1467,19 +1467,19 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>16.22005926784346</v>
+        <v>16.30140293573242</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>2.124603604416256</v>
+        <v>2.095313058753793</v>
       </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32">
-        <v>30.26856216431271</v>
+        <v>30.21801989310798</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -1500,19 +1500,19 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>21340.29250062991</v>
+        <v>21368.39305305418</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>2504.644200129112</v>
+        <v>2475.047938190708</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33">
-        <v>65595.10613684659</v>
+        <v>63661.14967061536</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -1531,19 +1531,19 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>21340.29250062991</v>
+        <v>21368.39305305418</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>2504.644200129112</v>
+        <v>2475.047938190708</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>65595.10613684659</v>
+        <v>63661.14967061536</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -1564,19 +1564,19 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0.3244011853568692</v>
+        <v>0.3260280587146485</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>0.04249207208832512</v>
+        <v>0.04190626117507586</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>0.6053712432862542</v>
+        <v>0.6043603978621596</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -1657,28 +1657,28 @@
         <v>25</v>
       </c>
       <c r="D2">
-        <v>0.03876872444753825</v>
+        <v>0.03194371080825167</v>
       </c>
       <c r="E2">
-        <v>0.04800538629882475</v>
+        <v>0.0509442374134374</v>
       </c>
       <c r="F2">
-        <v>0.5346714068466113</v>
+        <v>0.5464791261875996</v>
       </c>
       <c r="G2">
-        <v>0.1219120516405958</v>
+        <v>0.1295974527834644</v>
       </c>
       <c r="H2">
-        <v>0.09119073893646207</v>
+        <v>0.09449469558999908</v>
       </c>
       <c r="I2">
-        <v>0.1780411944075622</v>
+        <v>0.1779901389811348</v>
       </c>
       <c r="J2">
-        <v>0.9978035307134157</v>
+        <v>0.9961050319570591</v>
       </c>
       <c r="K2">
-        <v>0.01678424002911028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1690,28 +1690,28 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>0.4455420140321286</v>
+        <v>0.367106874213192</v>
       </c>
       <c r="E3">
-        <v>0.5516925511674103</v>
+        <v>0.5854667251492481</v>
       </c>
       <c r="F3">
-        <v>6.144606995625757</v>
+        <v>6.280304910150363</v>
       </c>
       <c r="G3">
-        <v>1.40105050647827</v>
+        <v>1.489373482088985</v>
       </c>
       <c r="H3">
-        <v>1.047991804368205</v>
+        <v>1.085961882637964</v>
       </c>
       <c r="I3">
-        <v>2.046103746445752</v>
+        <v>2.045517001902518</v>
       </c>
       <c r="J3">
-        <v>11.46706271659792</v>
+        <v>11.44754305048762</v>
       </c>
       <c r="K3">
-        <v>0.1928896091664762</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1723,28 +1723,28 @@
         <v>25</v>
       </c>
       <c r="D4">
-        <v>0.03319944927213665</v>
+        <v>0.02735487488058677</v>
       </c>
       <c r="E4">
-        <v>0.04110922940923212</v>
+        <v>0.04362590334907179</v>
       </c>
       <c r="F4">
-        <v>0.4578638194012893</v>
+        <v>0.4679753148107201</v>
       </c>
       <c r="G4">
-        <v>0.1043989203096175</v>
+        <v>0.1109802842573521</v>
       </c>
       <c r="H4">
-        <v>0.0780908413818595</v>
+        <v>0.08092017205702454</v>
       </c>
       <c r="I4">
-        <v>0.1524648975769903</v>
+        <v>0.1524211764573533</v>
       </c>
       <c r="J4">
-        <v>0.8544652467559417</v>
+        <v>0.8530107438259639</v>
       </c>
       <c r="K4">
-        <v>0.01437311991452932</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1756,28 +1756,28 @@
         <v>33</v>
       </c>
       <c r="D5">
-        <v>0.2227710070160643</v>
+        <v>0.183553437106596</v>
       </c>
       <c r="E5">
-        <v>0.2758462755837052</v>
+        <v>0.2927333625746241</v>
       </c>
       <c r="F5">
-        <v>3.072303497812878</v>
+        <v>3.140152455075182</v>
       </c>
       <c r="G5">
-        <v>0.7005252532391348</v>
+        <v>0.7446867410444927</v>
       </c>
       <c r="H5">
-        <v>0.5239959021841025</v>
+        <v>0.5429809413189819</v>
       </c>
       <c r="I5">
-        <v>1.023051873222876</v>
+        <v>1.022758500951259</v>
       </c>
       <c r="J5">
-        <v>5.73353135829896</v>
+        <v>5.723771525243809</v>
       </c>
       <c r="K5">
-        <v>0.09644480458323811</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1789,28 +1789,28 @@
         <v>28</v>
       </c>
       <c r="D6">
-        <v>1440.882873379904</v>
+        <v>1210.351364280878</v>
       </c>
       <c r="E6">
-        <v>1668.318274730249</v>
+        <v>1761.01829623186</v>
       </c>
       <c r="F6">
-        <v>25016.38365066085</v>
+        <v>25579.5987289314</v>
       </c>
       <c r="G6">
-        <v>5671.439862892332</v>
+        <v>6010.348834023017</v>
       </c>
       <c r="H6">
-        <v>3651.575350506165</v>
+        <v>3689.049339477815</v>
       </c>
       <c r="I6">
-        <v>8210.605103010908</v>
+        <v>8210.605103010463</v>
       </c>
       <c r="J6">
-        <v>52921.48610283091</v>
+        <v>52921.71198983486</v>
       </c>
       <c r="K6">
-        <v>801.9924377783246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1820,28 +1820,28 @@
         <v>29</v>
       </c>
       <c r="D7">
-        <v>1440.882873379904</v>
+        <v>1210.351364280878</v>
       </c>
       <c r="E7">
-        <v>1668.318274730249</v>
+        <v>1761.01829623186</v>
       </c>
       <c r="F7">
-        <v>25016.38365066085</v>
+        <v>25579.5987289314</v>
       </c>
       <c r="G7">
-        <v>5671.439862892332</v>
+        <v>6010.348834023017</v>
       </c>
       <c r="H7">
-        <v>3651.575350506165</v>
+        <v>3689.049339477815</v>
       </c>
       <c r="I7">
-        <v>8210.605103010908</v>
+        <v>8210.605103010463</v>
       </c>
       <c r="J7">
-        <v>52921.48610283091</v>
+        <v>52921.71198983486</v>
       </c>
       <c r="K7">
-        <v>801.9924377783246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1853,28 +1853,28 @@
         <v>25</v>
       </c>
       <c r="D8">
-        <v>0.005569275175401608</v>
+        <v>0.0045888359276649</v>
       </c>
       <c r="E8">
-        <v>0.006896156889592629</v>
+        <v>0.007318334064365602</v>
       </c>
       <c r="F8">
-        <v>0.07680758744532196</v>
+        <v>0.07850381137687955</v>
       </c>
       <c r="G8">
-        <v>0.01751313133097837</v>
+        <v>0.01861716852611232</v>
       </c>
       <c r="H8">
-        <v>0.01309989755460256</v>
+        <v>0.01357452353297455</v>
       </c>
       <c r="I8">
-        <v>0.0255762968305719</v>
+        <v>0.02556896252378147</v>
       </c>
       <c r="J8">
-        <v>0.143338283957474</v>
+        <v>0.1430942881310952</v>
       </c>
       <c r="K8">
-        <v>0.002411120114580953</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1888,28 +1888,28 @@
         <v>25</v>
       </c>
       <c r="D9">
-        <v>0.0555976789627078</v>
+        <v>0.02873578756825177</v>
       </c>
       <c r="E9">
-        <v>0.2302210280517785</v>
+        <v>0.2315605553811362</v>
       </c>
       <c r="F9">
-        <v>0.3221185594821037</v>
+        <v>0.3391852684354407</v>
       </c>
       <c r="G9">
-        <v>0.1347730274731471</v>
+        <v>0.1354877710138846</v>
       </c>
       <c r="H9">
-        <v>0.07644497927734294</v>
+        <v>0.07644497927734295</v>
       </c>
       <c r="I9">
-        <v>0.08607341446099116</v>
+        <v>0.08652506703522779</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0.007176229328296224</v>
+        <v>0.01435245865659245</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1921,28 +1921,28 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>0.679710278998644</v>
+        <v>0.3513098127417026</v>
       </c>
       <c r="E10">
-        <v>2.814570718201933</v>
+        <v>2.830947130162849</v>
       </c>
       <c r="F10">
-        <v>3.938065401670475</v>
+        <v>4.146714714388049</v>
       </c>
       <c r="G10">
-        <v>1.647669719570667</v>
+        <v>1.656407827717466</v>
       </c>
       <c r="H10">
-        <v>0.9345792695321121</v>
+        <v>0.9345792695321122</v>
       </c>
       <c r="I10">
-        <v>1.052291851911453</v>
+        <v>1.05781353740215</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0.08773310199093452</v>
+        <v>0.175466203981869</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1954,28 +1954,28 @@
         <v>25</v>
       </c>
       <c r="D11">
-        <v>0.04132376310373628</v>
+        <v>0.02135828150067601</v>
       </c>
       <c r="E11">
-        <v>0.1711150429695379</v>
+        <v>0.1721106656477163</v>
       </c>
       <c r="F11">
-        <v>0.2394191860470237</v>
+        <v>0.2521042594332916</v>
       </c>
       <c r="G11">
-        <v>0.1001719633621631</v>
+        <v>0.1007032066318178</v>
       </c>
       <c r="H11">
-        <v>0.05681881461716858</v>
+        <v>0.0568188146171686</v>
       </c>
       <c r="I11">
-        <v>0.06397528557085065</v>
+        <v>0.06431098274978263</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0.005333834186486599</v>
+        <v>0.0106676683729732</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1987,28 +1987,28 @@
         <v>33</v>
       </c>
       <c r="D12">
-        <v>0.4757971952990508</v>
+        <v>0.2459168689191918</v>
       </c>
       <c r="E12">
-        <v>1.970199502741353</v>
+        <v>1.981662991113994</v>
       </c>
       <c r="F12">
-        <v>2.756645781169333</v>
+        <v>2.902700300071634</v>
       </c>
       <c r="G12">
-        <v>1.153368803699467</v>
+        <v>1.159485479402226</v>
       </c>
       <c r="H12">
-        <v>0.6542054886724784</v>
+        <v>0.6542054886724785</v>
       </c>
       <c r="I12">
-        <v>0.7366042963380171</v>
+        <v>0.7404694761815053</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0.06141317139365416</v>
+        <v>0.1228263427873083</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2020,28 +2020,28 @@
         <v>28</v>
       </c>
       <c r="D13">
-        <v>1178.295204977841</v>
+        <v>622.5209881782812</v>
       </c>
       <c r="E13">
-        <v>4875.826628509128</v>
+        <v>4875.826628508413</v>
       </c>
       <c r="F13">
-        <v>6978.23846934555</v>
+        <v>7383.721415914494</v>
       </c>
       <c r="G13">
-        <v>2843.819678633008</v>
+        <v>2843.819678633365</v>
       </c>
       <c r="H13">
-        <v>1677.601389325355</v>
+        <v>1672.429602827759</v>
       </c>
       <c r="I13">
-        <v>1812.245461588044</v>
+        <v>1812.245461588006</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>163.9731676210566</v>
+        <v>319.4362243489834</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2051,28 +2051,28 @@
         <v>29</v>
       </c>
       <c r="D14">
-        <v>1178.295204977841</v>
+        <v>622.5209881782812</v>
       </c>
       <c r="E14">
-        <v>4875.826628509128</v>
+        <v>4875.826628508413</v>
       </c>
       <c r="F14">
-        <v>6978.23846934555</v>
+        <v>7383.721415914494</v>
       </c>
       <c r="G14">
-        <v>2843.819678633008</v>
+        <v>2843.819678633365</v>
       </c>
       <c r="H14">
-        <v>1677.601389325355</v>
+        <v>1672.429602827759</v>
       </c>
       <c r="I14">
-        <v>1812.245461588044</v>
+        <v>1812.245461588006</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
-        <v>163.9731676210566</v>
+        <v>319.4362243489834</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2084,28 +2084,28 @@
         <v>25</v>
       </c>
       <c r="D15">
-        <v>0.01427391585897153</v>
+        <v>0.007377506067575756</v>
       </c>
       <c r="E15">
-        <v>0.0591059850822406</v>
+        <v>0.05944988973341982</v>
       </c>
       <c r="F15">
-        <v>0.08269937343507998</v>
+        <v>0.08708100900214905</v>
       </c>
       <c r="G15">
-        <v>0.03460106411098401</v>
+        <v>0.03478456438206679</v>
       </c>
       <c r="H15">
-        <v>0.01962616466017435</v>
+        <v>0.01962616466017436</v>
       </c>
       <c r="I15">
-        <v>0.02209812889014051</v>
+        <v>0.02221408428544516</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>0.001842395141809625</v>
+        <v>0.00368479028361925</v>
       </c>
     </row>
   </sheetData>
@@ -2173,28 +2173,28 @@
         <v>25</v>
       </c>
       <c r="D2">
-        <v>0.1400526404278749</v>
+        <v>0.1624709635738654</v>
       </c>
       <c r="E2">
-        <v>0.4224960469206524</v>
+        <v>0.4244081817295711</v>
       </c>
       <c r="F2">
-        <v>0.8235384286302335</v>
+        <v>0.8185187603881047</v>
       </c>
       <c r="G2">
-        <v>0.1732370814004598</v>
+        <v>0.1660204711648393</v>
       </c>
       <c r="H2">
-        <v>0.2227964332028733</v>
+        <v>0.1947745285091281</v>
       </c>
       <c r="I2">
-        <v>0.1453782277490439</v>
+        <v>0.1563164854880773</v>
       </c>
       <c r="J2">
-        <v>0.12094700951039</v>
+        <v>0.120206372552679</v>
       </c>
       <c r="K2">
-        <v>0.1271533162590088</v>
+        <v>0.1326061098784412</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2206,28 +2206,28 @@
         <v>29</v>
       </c>
       <c r="D3">
-        <v>8.335056518501707</v>
+        <v>9.669254787816703</v>
       </c>
       <c r="E3">
-        <v>25.14432015825309</v>
+        <v>25.25811845334157</v>
       </c>
       <c r="F3">
-        <v>49.01185244933719</v>
+        <v>48.71311321547164</v>
       </c>
       <c r="G3">
-        <v>10.30998673185831</v>
+        <v>9.880499261988927</v>
       </c>
       <c r="H3">
-        <v>13.25944914135966</v>
+        <v>11.59176077315131</v>
       </c>
       <c r="I3">
-        <v>8.652002141094377</v>
+        <v>9.302978775238831</v>
       </c>
       <c r="J3">
-        <v>7.198008955297213</v>
+        <v>7.153930879486918</v>
       </c>
       <c r="K3">
-        <v>7.567369485472553</v>
+        <v>7.891885630707965</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2239,28 +2239,28 @@
         <v>25</v>
       </c>
       <c r="D4">
-        <v>0.1233825273908715</v>
+        <v>0.143132453998232</v>
       </c>
       <c r="E4">
-        <v>0.3722074066041462</v>
+        <v>0.373891944822888</v>
       </c>
       <c r="F4">
-        <v>0.7255147237315591</v>
+        <v>0.7210925339571614</v>
       </c>
       <c r="G4">
-        <v>0.1526171079367432</v>
+        <v>0.1462594726408614</v>
       </c>
       <c r="H4">
-        <v>0.196277534920154</v>
+        <v>0.1715910069628255</v>
       </c>
       <c r="I4">
-        <v>0.1280742234668552</v>
+        <v>0.1377105279375996</v>
       </c>
       <c r="J4">
-        <v>0.1065509915997956</v>
+        <v>0.1058985107937052</v>
       </c>
       <c r="K4">
-        <v>0.1120185772880637</v>
+        <v>0.1168223386170253</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2272,28 +2272,28 @@
         <v>33</v>
       </c>
       <c r="D5">
-        <v>1.258593534293758</v>
+        <v>1.460057472960322</v>
       </c>
       <c r="E5">
-        <v>3.796792343896217</v>
+        <v>3.813975886454577</v>
       </c>
       <c r="F5">
-        <v>7.400789719849915</v>
+        <v>7.355680095536217</v>
       </c>
       <c r="G5">
-        <v>1.556807996510605</v>
+        <v>1.491955388560328</v>
       </c>
       <c r="H5">
-        <v>2.002176820345309</v>
+        <v>1.750355876745847</v>
       </c>
       <c r="I5">
-        <v>1.306452323305251</v>
+        <v>1.404749795061063</v>
       </c>
       <c r="J5">
-        <v>1.086899352249879</v>
+        <v>1.080243562802525</v>
       </c>
       <c r="K5">
-        <v>1.142672792306356</v>
+        <v>1.191674730236903</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2305,28 +2305,28 @@
         <v>28</v>
       </c>
       <c r="D6">
-        <v>3091.224844307188</v>
+        <v>3789.684929998478</v>
       </c>
       <c r="E6">
-        <v>8280.055481168036</v>
+        <v>9149.117594285864</v>
       </c>
       <c r="F6">
-        <v>16601.07065993633</v>
+        <v>15607.64306417518</v>
       </c>
       <c r="G6">
-        <v>2658.25987156959</v>
+        <v>3138.24351013341</v>
       </c>
       <c r="H6">
-        <v>4190.750276111694</v>
+        <v>4060.208312910208</v>
       </c>
       <c r="I6">
-        <v>3498.574897695757</v>
+        <v>3698.925677846693</v>
       </c>
       <c r="J6">
-        <v>2242.855542040239</v>
+        <v>2499.679847291245</v>
       </c>
       <c r="K6">
-        <v>2771.422476755823</v>
+        <v>2502.087598668261</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2336,28 +2336,28 @@
         <v>29</v>
       </c>
       <c r="D7">
-        <v>3091.224844307188</v>
+        <v>3789.684929998478</v>
       </c>
       <c r="E7">
-        <v>8280.055481168036</v>
+        <v>9149.117594285864</v>
       </c>
       <c r="F7">
-        <v>16601.07065993633</v>
+        <v>15607.64306417518</v>
       </c>
       <c r="G7">
-        <v>2658.25987156959</v>
+        <v>3138.24351013341</v>
       </c>
       <c r="H7">
-        <v>4190.750276111694</v>
+        <v>4060.208312910208</v>
       </c>
       <c r="I7">
-        <v>3498.574897695757</v>
+        <v>3698.925677846693</v>
       </c>
       <c r="J7">
-        <v>2242.855542040239</v>
+        <v>2499.679847291245</v>
       </c>
       <c r="K7">
-        <v>2771.422476755823</v>
+        <v>2502.087598668261</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2369,28 +2369,28 @@
         <v>28</v>
       </c>
       <c r="D8">
-        <v>2788.468078772076</v>
+        <v>3418.975687521916</v>
       </c>
       <c r="E8">
-        <v>7469.582912477345</v>
+        <v>8253.680930830844</v>
       </c>
       <c r="F8">
-        <v>14976.5185007519</v>
+        <v>14079.95958517545</v>
       </c>
       <c r="G8">
-        <v>2398.272229410911</v>
+        <v>2831.24643201459</v>
       </c>
       <c r="H8">
-        <v>3780.679476161116</v>
+        <v>3663.021466788304</v>
       </c>
       <c r="I8">
-        <v>3156.194685132692</v>
+        <v>3337.246725882045</v>
       </c>
       <c r="J8">
-        <v>2023.361922834928</v>
+        <v>2254.895650429553</v>
       </c>
       <c r="K8">
-        <v>2500.205593292352</v>
+        <v>2257.117500010898</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2400,28 +2400,28 @@
         <v>29</v>
       </c>
       <c r="D9">
-        <v>2788.468078772076</v>
+        <v>3418.975687521916</v>
       </c>
       <c r="E9">
-        <v>7469.582912477345</v>
+        <v>8253.680930830844</v>
       </c>
       <c r="F9">
-        <v>14976.5185007519</v>
+        <v>14079.95958517545</v>
       </c>
       <c r="G9">
-        <v>2398.272229410911</v>
+        <v>2831.24643201459</v>
       </c>
       <c r="H9">
-        <v>3780.679476161116</v>
+        <v>3663.021466788304</v>
       </c>
       <c r="I9">
-        <v>3156.194685132692</v>
+        <v>3337.246725882045</v>
       </c>
       <c r="J9">
-        <v>2023.361922834928</v>
+        <v>2254.895650429553</v>
       </c>
       <c r="K9">
-        <v>2500.205593292352</v>
+        <v>2257.117500010898</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2433,28 +2433,28 @@
         <v>25</v>
       </c>
       <c r="D10">
-        <v>0.01667011303700341</v>
+        <v>0.01933850957563341</v>
       </c>
       <c r="E10">
-        <v>0.05028864031650618</v>
+        <v>0.05051623690668315</v>
       </c>
       <c r="F10">
-        <v>0.09802370489867439</v>
+        <v>0.09742622643094327</v>
       </c>
       <c r="G10">
-        <v>0.02061997346371663</v>
+        <v>0.01976099852397785</v>
       </c>
       <c r="H10">
-        <v>0.02651889828271932</v>
+        <v>0.02318352154630261</v>
       </c>
       <c r="I10">
-        <v>0.01730400428218875</v>
+        <v>0.01860595755047766</v>
       </c>
       <c r="J10">
-        <v>0.01439601791059443</v>
+        <v>0.01430786175897384</v>
       </c>
       <c r="K10">
-        <v>0.01513473897094511</v>
+        <v>0.01578377126141593</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2531,25 +2531,25 @@
         <v>28</v>
       </c>
       <c r="D13">
-        <v>6693.596748365845</v>
+        <v>6993.704075132623</v>
       </c>
       <c r="E13">
-        <v>3944.855259240243</v>
+        <v>3736.598651770728</v>
       </c>
       <c r="F13">
-        <v>402.3563201570678</v>
+        <v>403.2811522543923</v>
       </c>
       <c r="G13">
-        <v>8596.819655444644</v>
+        <v>8565.721379696812</v>
       </c>
       <c r="H13">
-        <v>3197.449763087371</v>
+        <v>3294.445506129176</v>
       </c>
       <c r="I13">
-        <v>9583.172127142336</v>
+        <v>9483.273118358264</v>
       </c>
       <c r="J13">
-        <v>293.3817569641672</v>
+        <v>292.1979935356568</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2559,25 +2559,25 @@
         <v>29</v>
       </c>
       <c r="D14">
-        <v>6693.596748365845</v>
+        <v>6993.704075132623</v>
       </c>
       <c r="E14">
-        <v>3944.855259240243</v>
+        <v>3736.598651770728</v>
       </c>
       <c r="F14">
-        <v>402.3563201570678</v>
+        <v>403.2811522543923</v>
       </c>
       <c r="G14">
-        <v>8596.819655444644</v>
+        <v>8565.721379696812</v>
       </c>
       <c r="H14">
-        <v>3197.449763087371</v>
+        <v>3294.445506129176</v>
       </c>
       <c r="I14">
-        <v>9583.172127142336</v>
+        <v>9483.273118358264</v>
       </c>
       <c r="J14">
-        <v>293.3817569641672</v>
+        <v>292.1979935356568</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2589,25 +2589,25 @@
         <v>28</v>
       </c>
       <c r="D15">
-        <v>5183.358089453864</v>
+        <v>5415.758024884561</v>
       </c>
       <c r="E15">
-        <v>3054.798323382123</v>
+        <v>2893.524385113345</v>
       </c>
       <c r="F15">
-        <v>311.57322536639</v>
+        <v>312.2908190183483</v>
       </c>
       <c r="G15">
-        <v>6657.183557964673</v>
+        <v>6633.091938915016</v>
       </c>
       <c r="H15">
-        <v>2476.02360436029</v>
+        <v>2551.135833887887</v>
       </c>
       <c r="I15">
-        <v>7420.962026660994</v>
+        <v>7343.598682297125</v>
       </c>
       <c r="J15">
-        <v>227.18123059227</v>
+        <v>226.2637240085259</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2617,25 +2617,25 @@
         <v>29</v>
       </c>
       <c r="D16">
-        <v>5183.358089453864</v>
+        <v>5415.758024884561</v>
       </c>
       <c r="E16">
-        <v>3054.798323382123</v>
+        <v>2893.524385113345</v>
       </c>
       <c r="F16">
-        <v>311.57322536639</v>
+        <v>312.2908190183483</v>
       </c>
       <c r="G16">
-        <v>6657.183557964673</v>
+        <v>6633.091938915016</v>
       </c>
       <c r="H16">
-        <v>2476.02360436029</v>
+        <v>2551.135833887887</v>
       </c>
       <c r="I16">
-        <v>7420.962026660994</v>
+        <v>7343.598682297125</v>
       </c>
       <c r="J16">
-        <v>227.18123059227</v>
+        <v>226.2637240085259</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2682,19 +2682,19 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0.02884557953110124</v>
+        <v>0.0290260768043454</v>
       </c>
       <c r="F18">
-        <v>0.05711290787108168</v>
+        <v>0.05690480499572455</v>
       </c>
       <c r="G18">
-        <v>0.01689726295966742</v>
+        <v>0.01683951924595331</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0.0107956130367463</v>
+        <v>0.01086206981838269</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -2712,16 +2712,16 @@
         <v>27</v>
       </c>
       <c r="E19">
-        <v>2128.338550005437</v>
+        <v>2141.65633772408</v>
       </c>
       <c r="F19">
-        <v>4214.011488098935</v>
+        <v>4198.65685216548</v>
       </c>
       <c r="G19">
-        <v>1246.745488606454</v>
+        <v>1242.48493382073</v>
       </c>
       <c r="I19">
-        <v>796.5421312570604</v>
+        <v>801.4455699317286</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -2736,16 +2736,16 @@
         <v>25</v>
       </c>
       <c r="E20">
-        <v>0.007562194031046864</v>
+        <v>0.007609513427104607</v>
       </c>
       <c r="F20">
-        <v>0.01497279299009233</v>
+        <v>0.01491823647406974</v>
       </c>
       <c r="G20">
-        <v>0.00442980807360288</v>
+        <v>0.004414669907746011</v>
       </c>
       <c r="I20">
-        <v>0.002830191724175697</v>
+        <v>0.002847614119065403</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -2760,16 +2760,16 @@
         <v>33</v>
       </c>
       <c r="E21">
-        <v>0.08513354200021749</v>
+        <v>0.08566625350896319</v>
       </c>
       <c r="F21">
-        <v>0.1685604595239574</v>
+        <v>0.1679462740866192</v>
       </c>
       <c r="G21">
-        <v>0.04986981954425816</v>
+        <v>0.04969939735282919</v>
       </c>
       <c r="I21">
-        <v>0.03186168525028242</v>
+        <v>0.03205782279726915</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -2784,16 +2784,16 @@
         <v>26</v>
       </c>
       <c r="E22">
-        <v>6128.774370447756</v>
+        <v>6173.224631484071</v>
       </c>
       <c r="F22">
-        <v>12496.99786693265</v>
+        <v>12516.62093909624</v>
       </c>
       <c r="G22">
-        <v>19089.99651923593</v>
+        <v>19003.52890553276</v>
       </c>
       <c r="I22">
-        <v>2294.69654373727</v>
+        <v>2309.68397578331</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -2806,16 +2806,16 @@
         <v>27</v>
       </c>
       <c r="E23">
-        <v>6128.774370447756</v>
+        <v>6173.224631484071</v>
       </c>
       <c r="F23">
-        <v>12496.99786693265</v>
+        <v>12516.62093909624</v>
       </c>
       <c r="G23">
-        <v>19089.99651923593</v>
+        <v>19003.52890553276</v>
       </c>
       <c r="I23">
-        <v>2294.69654373727</v>
+        <v>2309.68397578331</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -2830,19 +2830,19 @@
         <v>26</v>
       </c>
       <c r="E24">
-        <v>6128.774370447756</v>
+        <v>6173.224631484794</v>
       </c>
       <c r="F24">
-        <v>12496.99786693265</v>
+        <v>12516.62093909638</v>
       </c>
       <c r="G24">
-        <v>19089.99651923593</v>
+        <v>19003.52890552734</v>
       </c>
       <c r="I24">
-        <v>2294.696543737271</v>
+        <v>2309.683975783427</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>9.477513218669742E-11</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2852,19 +2852,19 @@
         <v>27</v>
       </c>
       <c r="E25">
-        <v>6128.774370447756</v>
+        <v>6173.224631484794</v>
       </c>
       <c r="F25">
-        <v>12496.99786693265</v>
+        <v>12516.62093909638</v>
       </c>
       <c r="G25">
-        <v>19089.99651923593</v>
+        <v>19003.52890552734</v>
       </c>
       <c r="I25">
-        <v>2294.696543737271</v>
+        <v>2309.683975783427</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>9.477513218669742E-11</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2876,16 +2876,16 @@
         <v>25</v>
       </c>
       <c r="E26">
-        <v>0.02128338550005437</v>
+        <v>0.0214165633772408</v>
       </c>
       <c r="F26">
-        <v>0.04214011488098935</v>
+        <v>0.0419865685216548</v>
       </c>
       <c r="G26">
-        <v>0.01246745488606454</v>
+        <v>0.0124248493382073</v>
       </c>
       <c r="I26">
-        <v>0.007965421312570605</v>
+        <v>0.008014455699317287</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -2905,19 +2905,19 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0.6184110518039891</v>
+        <v>0.6183213061631192</v>
       </c>
       <c r="F27">
-        <v>0.6473868078187776</v>
+        <v>0.641456130516345</v>
       </c>
       <c r="G27">
-        <v>0.1714787187766951</v>
+        <v>0.1784384830976239</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0.2116680116609342</v>
+        <v>0.2115560051637351</v>
       </c>
       <c r="J27">
         <v>0.6326083603512803</v>
@@ -2935,16 +2935,16 @@
         <v>32</v>
       </c>
       <c r="E28">
-        <v>1066.647060569712</v>
+        <v>1066.492265593533</v>
       </c>
       <c r="F28">
-        <v>1116.624991738308</v>
+        <v>1106.395647528865</v>
       </c>
       <c r="G28">
-        <v>295.7697324455258</v>
+        <v>307.7740653783234</v>
       </c>
       <c r="I28">
-        <v>365.0889837692168</v>
+        <v>364.8957928476549</v>
       </c>
       <c r="J28">
         <v>1091.134846461949</v>
@@ -2959,16 +2959,16 @@
         <v>25</v>
       </c>
       <c r="E29">
-        <v>0.01042222727925344</v>
+        <v>0.01042071477480557</v>
       </c>
       <c r="F29">
-        <v>0.01091056252794178</v>
+        <v>0.0108106114248922</v>
       </c>
       <c r="G29">
-        <v>0.002889971282745392</v>
+        <v>0.003007265831979531</v>
       </c>
       <c r="I29">
-        <v>0.003567290912480574</v>
+        <v>0.003565403240571806</v>
       </c>
       <c r="J29">
         <v>0.01066149786796934</v>
@@ -2983,16 +2983,16 @@
         <v>33</v>
       </c>
       <c r="E30">
-        <v>0.1173311766626683</v>
+        <v>0.1173141492152886</v>
       </c>
       <c r="F30">
-        <v>0.1228287490912139</v>
+        <v>0.1217035212281751</v>
       </c>
       <c r="G30">
-        <v>0.03253467056900784</v>
+        <v>0.03385514719161558</v>
       </c>
       <c r="I30">
-        <v>0.04015978821461386</v>
+        <v>0.04013853721324204</v>
       </c>
       <c r="J30">
         <v>0.1200248331108144</v>
@@ -3007,19 +3007,19 @@
         <v>31</v>
       </c>
       <c r="E31">
-        <v>8291.901496935725</v>
+        <v>8260.477444326514</v>
       </c>
       <c r="F31">
-        <v>9287.843176545975</v>
+        <v>9143.788730841476</v>
       </c>
       <c r="G31">
-        <v>3001.080106289332</v>
+        <v>3131.560023785447</v>
       </c>
       <c r="I31">
-        <v>2901.933104017665</v>
+        <v>2933.743650354726</v>
       </c>
       <c r="J31">
-        <v>11286.8718857521</v>
+        <v>11485.86800871523</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -3029,19 +3029,19 @@
         <v>32</v>
       </c>
       <c r="E32">
-        <v>8291.901496935725</v>
+        <v>8260.477444326514</v>
       </c>
       <c r="F32">
-        <v>9287.843176545975</v>
+        <v>9143.788730841476</v>
       </c>
       <c r="G32">
-        <v>3001.080106289332</v>
+        <v>3131.560023785447</v>
       </c>
       <c r="I32">
-        <v>2901.933104017665</v>
+        <v>2933.743650354726</v>
       </c>
       <c r="J32">
-        <v>11286.8718857521</v>
+        <v>11485.86800871523</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -3053,19 +3053,19 @@
         <v>31</v>
       </c>
       <c r="E33">
-        <v>8291.901496935694</v>
+        <v>8260.477444326329</v>
       </c>
       <c r="F33">
-        <v>9287.84317654599</v>
+        <v>9143.788730840983</v>
       </c>
       <c r="G33">
-        <v>3001.080106289335</v>
+        <v>3131.56002378552</v>
       </c>
       <c r="I33">
-        <v>2901.933104017664</v>
+        <v>2933.743650354754</v>
       </c>
       <c r="J33">
-        <v>11286.87188575211</v>
+        <v>11485.86800871513</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3075,19 +3075,19 @@
         <v>32</v>
       </c>
       <c r="E34">
-        <v>8291.901496935694</v>
+        <v>8260.477444326329</v>
       </c>
       <c r="F34">
-        <v>9287.84317654599</v>
+        <v>9143.788730840983</v>
       </c>
       <c r="G34">
-        <v>3001.080106289335</v>
+        <v>3131.56002378552</v>
       </c>
       <c r="I34">
-        <v>2901.933104017664</v>
+        <v>2933.743650354754</v>
       </c>
       <c r="J34">
-        <v>11286.87188575211</v>
+        <v>11485.86800871513</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3099,16 +3099,16 @@
         <v>25</v>
       </c>
       <c r="E35">
-        <v>0.6079888245247357</v>
+        <v>0.6079005913883136</v>
       </c>
       <c r="F35">
-        <v>0.6364762452908358</v>
+        <v>0.6306455190914528</v>
       </c>
       <c r="G35">
-        <v>0.1685887474939497</v>
+        <v>0.1754312172656443</v>
       </c>
       <c r="I35">
-        <v>0.2081007207484536</v>
+        <v>0.2079906019231633</v>
       </c>
       <c r="J35">
         <v>0.621946862483311</v>
@@ -3135,7 +3135,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3190,10 +3190,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.01317987013689491</v>
+        <v>0.01324904725903324</v>
       </c>
       <c r="F2">
-        <v>0.004712027659101854</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3218,7 +3218,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.01317987013689491</v>
+        <v>0.01324904725903324</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3236,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.01561676288782131</v>
+        <v>0.01566801357122064</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3249,7 +3249,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>0.004712027659101854</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3298,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.006022992264144319</v>
+        <v>0.00591952639511153</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -3345,13 +3345,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.01561676288782131</v>
+        <v>0.01566801357122064</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.006022992264144319</v>
+        <v>0.00591952639511153</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3408,10 +3408,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>2.935252868268806</v>
+        <v>2.960444819193862</v>
       </c>
       <c r="F9">
-        <v>0.02519195092505555</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>1.150487160399343</v>
@@ -3430,7 +3430,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>2.935252868268806</v>
+        <v>2.960444819193862</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -3442,7 +3442,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>5.034689597557425</v>
+        <v>5.057330871341892</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3452,7 +3452,7 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>0.02519195092505555</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3474,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.2489952289920642</v>
+        <v>0.212690188930387</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -3497,10 +3497,10 @@
         <v>6</v>
       </c>
       <c r="E14">
-        <v>5.034689597557425</v>
+        <v>5.057330871341892</v>
       </c>
       <c r="G14">
-        <v>0.2489952289920642</v>
+        <v>0.212690188930387</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -3527,10 +3527,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0.008060207277284176</v>
+        <v>0.008129384399422507</v>
       </c>
       <c r="F16">
-        <v>6.282030550940359E-05</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0.002629852905118307</v>
@@ -3549,7 +3549,7 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>0.008060207277284176</v>
+        <v>0.008129384399422507</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -3561,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0.01139650026030436</v>
+        <v>0.01144775094370368</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -3571,7 +3571,7 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <v>6.282030550940359E-05</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -3593,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0.0007096124314672323</v>
+        <v>0.0006061465624344441</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -3616,10 +3616,10 @@
         <v>6</v>
       </c>
       <c r="E21">
-        <v>0.01139650026030436</v>
+        <v>0.01144775094370368</v>
       </c>
       <c r="G21">
-        <v>0.0007096124314672323</v>
+        <v>0.0006061465624344441</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -3649,7 +3649,7 @@
         <v>0.005119662859610734</v>
       </c>
       <c r="F23">
-        <v>0.00464920735359245</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0.004261773407459746</v>
@@ -3690,7 +3690,7 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <v>0.00464920735359245</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -3765,10 +3765,10 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.1571648551714621</v>
+        <v>0.157989765604503</v>
       </c>
       <c r="F30">
-        <v>0.05618910785270746</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <v>0.08217997901816528</v>
@@ -3787,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>0.1571648551714621</v>
+        <v>0.157989765604503</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -3799,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0.1862238589620688</v>
+        <v>0.186835003544696</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -3809,7 +3809,7 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <v>0.05618910785270746</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -3831,7 +3831,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>0.07182185386206631</v>
+        <v>0.07058806338061027</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -3854,10 +3854,10 @@
         <v>6</v>
       </c>
       <c r="E35">
-        <v>0.1862238589620688</v>
+        <v>0.186835003544696</v>
       </c>
       <c r="G35">
-        <v>0.07182185386206631</v>
+        <v>0.07058806338061027</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -3887,7 +3887,7 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -3928,7 +3928,7 @@
         <v>2</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -4003,13 +4003,13 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>146.9855847993173</v>
+        <v>196.0047602176767</v>
       </c>
       <c r="F44">
-        <v>15.93018630739932</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>7535.002679347434</v>
+        <v>7495.932987463812</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -4025,7 +4025,7 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>22348.61729256187</v>
+        <v>22699.92088372306</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -4037,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>2.668025538767781</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -4047,13 +4047,13 @@
         <v>2</v>
       </c>
       <c r="D46">
-        <v>183.0743379628314</v>
+        <v>0</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="K46">
-        <v>901.3448836354899</v>
+        <v>1453.124166487049</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -4069,163 +4069,111 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>113.4665725850904</v>
+        <v>142.6711758116724</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48">
-        <v>12.83789960351051</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>32278.26019852427</v>
+      </c>
+      <c r="G48">
+        <v>1199.558856360252</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C49" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>32043.53382336824</v>
-      </c>
-      <c r="G49">
-        <v>1407.590532925276</v>
+        <v>196.0047602176767</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>7495.932987463812</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>22699.92088372306</v>
       </c>
       <c r="F50">
-        <v>9.615423593131757</v>
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="1"/>
-      <c r="B51" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>146.9855847993173</v>
-      </c>
-      <c r="F51">
-        <v>15.93018630739932</v>
-      </c>
-      <c r="H51">
-        <v>7535.002679347434</v>
-      </c>
-      <c r="I51">
         <v>0</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>1453.124166487049</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>22348.61729256187</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="E52">
         <v>0</v>
       </c>
       <c r="I52">
         <v>0</v>
       </c>
       <c r="J52">
-        <v>2.668025538767781</v>
+        <v>142.6711758116724</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53">
-        <v>183.0743379628314</v>
+        <v>6</v>
       </c>
       <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="K53">
-        <v>901.3448836354899</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="I54">
-        <v>0</v>
-      </c>
-      <c r="J54">
-        <v>113.4665725850904</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55">
-        <v>12.83789960351051</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56">
-        <v>32043.53382336824</v>
-      </c>
-      <c r="G56">
-        <v>1407.590532925276</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>9.615423593131757</v>
+        <v>32278.26019852427</v>
+      </c>
+      <c r="G53">
+        <v>1199.558856360252</v>
       </c>
     </row>
   </sheetData>
@@ -4236,15 +4184,15 @@
     <mergeCell ref="A23:A29"/>
     <mergeCell ref="A30:A36"/>
     <mergeCell ref="A37:A43"/>
-    <mergeCell ref="A44:A57"/>
+    <mergeCell ref="A44:A53"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="B16:B22"/>
     <mergeCell ref="B23:B29"/>
     <mergeCell ref="B30:B36"/>
     <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="B51:B57"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>